<commit_message>
#7: Added new Joinpoint outputs by demo groups
</commit_message>
<xml_diff>
--- a/raw/Raw and Age-Adjusted National Mortality Rates by Non-Hispanic White vs. Non-Hispanic Black (2007 - 2020).xlsx
+++ b/raw/Raw and Age-Adjusted National Mortality Rates by Non-Hispanic White vs. Non-Hispanic Black (2007 - 2020).xlsx
@@ -1,27 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sameernd/Desktop/CJD_Epi/raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fe353eac81e08534/Desktop/CJD_Epi-master/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{A4CDC54E-3D12-984F-845E-15C4BBEA572A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:40009_{A4CDC54E-3D12-984F-845E-15C4BBEA572A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12496FEC-CC39-479F-BD5E-AFB0DC955645}"/>
   <bookViews>
-    <workbookView xWindow="4020" yWindow="500" windowWidth="28040" windowHeight="16440"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17664" windowHeight="8952" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mortality Rates" sheetId="1" r:id="rId1"/>
     <sheet name="Query Documentation" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Mortality Rates'!$D$1:$D$44</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="99">
   <si>
     <t>Notes</t>
   </si>
@@ -309,12 +312,21 @@
   </si>
   <si>
     <t>https://wonder.cdc.gov/controller/saved/D77/D326F027</t>
+  </si>
+  <si>
+    <t>Age Adjusted Rate Lower 95% Confidence Interval</t>
+  </si>
+  <si>
+    <t>Age Adjusted Rate Upper 95% Confidence Interval</t>
+  </si>
+  <si>
+    <t>Age Adjusted Rate Standard Error</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -871,6 +883,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1167,16 +1183,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:P44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="G23" sqref="A1:P44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1214,10 +1231,19 @@
         <v>11</v>
       </c>
       <c r="M1" t="s">
+        <v>96</v>
+      </c>
+      <c r="N1" t="s">
+        <v>97</v>
+      </c>
+      <c r="O1" t="s">
+        <v>98</v>
+      </c>
+      <c r="P1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>2007</v>
       </c>
@@ -1252,10 +1278,19 @@
         <v>15</v>
       </c>
       <c r="M2" s="1">
+        <v>2.5250000000000002E-2</v>
+      </c>
+      <c r="N2">
+        <v>8.5360000000000005E-2</v>
+      </c>
+      <c r="O2">
+        <v>1.43E-2</v>
+      </c>
+      <c r="P2" s="1">
         <v>2.3697000000000002E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>2007</v>
       </c>
@@ -1290,10 +1325,19 @@
         <v>0.10399</v>
       </c>
       <c r="M3" s="1">
+        <v>9.1149999999999995E-2</v>
+      </c>
+      <c r="N3">
+        <v>0.11683</v>
+      </c>
+      <c r="O3">
+        <v>6.5500000000000003E-3</v>
+      </c>
+      <c r="P3" s="1">
         <v>5.1540299999999997E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -1325,10 +1369,19 @@
         <v>9.5259999999999997E-2</v>
       </c>
       <c r="M4" s="1">
+        <v>8.3640000000000006E-2</v>
+      </c>
+      <c r="N4">
+        <v>0.10689</v>
+      </c>
+      <c r="O4">
+        <v>5.9300000000000004E-3</v>
+      </c>
+      <c r="P4" s="1">
         <v>5.391E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>2008</v>
       </c>
@@ -1363,10 +1416,19 @@
         <v>15</v>
       </c>
       <c r="M5" s="1">
+        <v>2.349E-2</v>
+      </c>
+      <c r="N5">
+        <v>7.5429999999999997E-2</v>
+      </c>
+      <c r="O5">
+        <v>1.244E-2</v>
+      </c>
+      <c r="P5" s="1">
         <v>3.1595999999999998E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>2008</v>
       </c>
@@ -1401,10 +1463,19 @@
         <v>0.11239</v>
       </c>
       <c r="M6" s="1">
+        <v>9.9169999999999994E-2</v>
+      </c>
+      <c r="N6">
+        <v>0.12561</v>
+      </c>
+      <c r="O6">
+        <v>6.7499999999999999E-3</v>
+      </c>
+      <c r="P6" s="1">
         <v>5.6674599999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1436,10 +1507,19 @@
         <v>0.11083999999999999</v>
       </c>
       <c r="M7" s="1">
+        <v>9.8119999999999999E-2</v>
+      </c>
+      <c r="N7">
+        <v>0.12354999999999999</v>
+      </c>
+      <c r="O7">
+        <v>6.4900000000000001E-3</v>
+      </c>
+      <c r="P7" s="1">
         <v>5.9834100000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>2009</v>
       </c>
@@ -1474,10 +1554,19 @@
         <v>15</v>
       </c>
       <c r="M8" s="1">
+        <v>2.4140000000000002E-2</v>
+      </c>
+      <c r="N8">
+        <v>8.1610000000000002E-2</v>
+      </c>
+      <c r="O8">
+        <v>1.371E-2</v>
+      </c>
+      <c r="P8" s="1">
         <v>2.5671000000000001E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>2009</v>
       </c>
@@ -1512,10 +1601,19 @@
         <v>0.10929</v>
       </c>
       <c r="M9" s="1">
+        <v>9.6149999999999999E-2</v>
+      </c>
+      <c r="N9">
+        <v>0.12242</v>
+      </c>
+      <c r="O9">
+        <v>6.7000000000000002E-3</v>
+      </c>
+      <c r="P9" s="1">
         <v>5.46998E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1547,10 +1645,19 @@
         <v>9.3960000000000002E-2</v>
       </c>
       <c r="M10" s="1">
+        <v>8.2720000000000002E-2</v>
+      </c>
+      <c r="N10">
+        <v>0.1052</v>
+      </c>
+      <c r="O10">
+        <v>5.7299999999999999E-3</v>
+      </c>
+      <c r="P10" s="1">
         <v>5.7266999999999998E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>2010</v>
       </c>
@@ -1585,10 +1692,19 @@
         <v>15</v>
       </c>
       <c r="M11" s="1">
+        <v>2.2919999999999999E-2</v>
+      </c>
+      <c r="N11">
+        <v>7.7469999999999997E-2</v>
+      </c>
+      <c r="O11">
+        <v>1.2619999999999999E-2</v>
+      </c>
+      <c r="P11" s="1">
         <v>3.3570000000000002E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>2010</v>
       </c>
@@ -1623,10 +1739,19 @@
         <v>0.11508</v>
       </c>
       <c r="M12" s="1">
+        <v>0.10218000000000001</v>
+      </c>
+      <c r="N12">
+        <v>0.12797</v>
+      </c>
+      <c r="O12">
+        <v>6.5799999999999999E-3</v>
+      </c>
+      <c r="P12" s="1">
         <v>6.1018999999999997E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1658,10 +1783,19 @@
         <v>0.10635</v>
       </c>
       <c r="M13" s="1">
+        <v>9.461E-2</v>
+      </c>
+      <c r="N13">
+        <v>0.1181</v>
+      </c>
+      <c r="O13">
+        <v>5.9899999999999997E-3</v>
+      </c>
+      <c r="P13" s="1">
         <v>6.4376000000000003E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>2011</v>
       </c>
@@ -1696,10 +1830,19 @@
         <v>6.7470000000000002E-2</v>
       </c>
       <c r="M14" s="1">
+        <v>4.1759999999999999E-2</v>
+      </c>
+      <c r="N14">
+        <v>0.10313</v>
+      </c>
+      <c r="O14">
+        <v>1.4659999999999999E-2</v>
+      </c>
+      <c r="P14" s="1">
         <v>4.9367999999999999E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>2011</v>
       </c>
@@ -1734,10 +1877,19 @@
         <v>0.11352</v>
       </c>
       <c r="M15" s="1">
+        <v>0.10094</v>
+      </c>
+      <c r="N15">
+        <v>0.12611</v>
+      </c>
+      <c r="O15">
+        <v>6.4200000000000004E-3</v>
+      </c>
+      <c r="P15" s="1">
         <v>6.3980999999999996E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1769,10 +1921,19 @@
         <v>0.11352</v>
       </c>
       <c r="M16" s="1">
+        <v>0.10134</v>
+      </c>
+      <c r="N16">
+        <v>0.12570000000000001</v>
+      </c>
+      <c r="O16">
+        <v>6.2100000000000002E-3</v>
+      </c>
+      <c r="P16" s="1">
         <v>6.8917900000000004E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>2012</v>
       </c>
@@ -1807,10 +1968,19 @@
         <v>15</v>
       </c>
       <c r="M17" s="1">
+        <v>2.793E-2</v>
+      </c>
+      <c r="N17">
+        <v>7.936E-2</v>
+      </c>
+      <c r="O17">
+        <v>1.2370000000000001E-2</v>
+      </c>
+      <c r="P17" s="1">
         <v>3.5544999999999999E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>2012</v>
       </c>
@@ -1845,10 +2015,19 @@
         <v>0.10324999999999999</v>
       </c>
       <c r="M18" s="1">
+        <v>9.0910000000000005E-2</v>
+      </c>
+      <c r="N18">
+        <v>0.11559</v>
+      </c>
+      <c r="O18">
+        <v>6.2899999999999996E-3</v>
+      </c>
+      <c r="P18" s="1">
         <v>5.8254300000000002E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1880,10 +2059,19 @@
         <v>0.10324999999999999</v>
       </c>
       <c r="M19" s="1">
+        <v>9.1399999999999995E-2</v>
+      </c>
+      <c r="N19">
+        <v>0.11509999999999999</v>
+      </c>
+      <c r="O19">
+        <v>6.0400000000000002E-3</v>
+      </c>
+      <c r="P19" s="1">
         <v>6.1808799999999997E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>2013</v>
       </c>
@@ -1918,10 +2106,19 @@
         <v>7.0800000000000002E-2</v>
       </c>
       <c r="M20" s="1">
+        <v>4.5359999999999998E-2</v>
+      </c>
+      <c r="N20">
+        <v>0.10534</v>
+      </c>
+      <c r="O20">
+        <v>1.455E-2</v>
+      </c>
+      <c r="P20" s="1">
         <v>5.1342999999999996E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>2013</v>
       </c>
@@ -1956,10 +2153,19 @@
         <v>0.12306</v>
       </c>
       <c r="M21" s="1">
+        <v>0.11003</v>
+      </c>
+      <c r="N21">
+        <v>0.1361</v>
+      </c>
+      <c r="O21">
+        <v>6.6499999999999997E-3</v>
+      </c>
+      <c r="P21" s="1">
         <v>7.0102700000000004E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -1991,10 +2197,19 @@
         <v>0.11434</v>
       </c>
       <c r="M22" s="1">
+        <v>0.10253</v>
+      </c>
+      <c r="N22">
+        <v>0.12615000000000001</v>
+      </c>
+      <c r="O22">
+        <v>6.0299999999999998E-3</v>
+      </c>
+      <c r="P22" s="1">
         <v>7.5236999999999998E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>2014</v>
       </c>
@@ -2029,10 +2244,19 @@
         <v>7.3899999999999993E-2</v>
       </c>
       <c r="M23" s="1">
+        <v>4.7829999999999998E-2</v>
+      </c>
+      <c r="N23">
+        <v>0.10909000000000001</v>
+      </c>
+      <c r="O23">
+        <v>1.469E-2</v>
+      </c>
+      <c r="P23" s="1">
         <v>5.1342999999999996E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>2014</v>
       </c>
@@ -2067,10 +2291,19 @@
         <v>0.10635</v>
       </c>
       <c r="M24" s="1">
+        <v>9.4729999999999995E-2</v>
+      </c>
+      <c r="N24">
+        <v>0.11797000000000001</v>
+      </c>
+      <c r="O24">
+        <v>5.9300000000000004E-3</v>
+      </c>
+      <c r="P24" s="1">
         <v>6.6548200000000002E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>18</v>
       </c>
@@ -2102,10 +2335,19 @@
         <v>0.10635</v>
       </c>
       <c r="M25" s="1">
+        <v>9.5170000000000005E-2</v>
+      </c>
+      <c r="N25">
+        <v>0.11754000000000001</v>
+      </c>
+      <c r="O25">
+        <v>5.7099999999999998E-3</v>
+      </c>
+      <c r="P25" s="1">
         <v>7.1682499999999996E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B26">
         <v>2015</v>
       </c>
@@ -2140,10 +2382,19 @@
         <v>7.3620000000000005E-2</v>
       </c>
       <c r="M26" s="1">
+        <v>4.7649999999999998E-2</v>
+      </c>
+      <c r="N26">
+        <v>0.10868999999999999</v>
+      </c>
+      <c r="O26">
+        <v>1.4579999999999999E-2</v>
+      </c>
+      <c r="P26" s="1">
         <v>5.3318000000000003E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="B27">
         <v>2015</v>
       </c>
@@ -2178,10 +2429,19 @@
         <v>0.12461</v>
       </c>
       <c r="M27" s="1">
+        <v>0.11189</v>
+      </c>
+      <c r="N27">
+        <v>0.13733000000000001</v>
+      </c>
+      <c r="O27">
+        <v>6.4900000000000001E-3</v>
+      </c>
+      <c r="P27" s="1">
         <v>7.4644500000000003E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>18</v>
       </c>
@@ -2213,10 +2473,19 @@
         <v>0.11589000000000001</v>
       </c>
       <c r="M28" s="1">
+        <v>0.10428</v>
+      </c>
+      <c r="N28">
+        <v>0.1275</v>
+      </c>
+      <c r="O28">
+        <v>5.9199999999999999E-3</v>
+      </c>
+      <c r="P28" s="1">
         <v>7.99763E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>2016</v>
       </c>
@@ -2251,10 +2520,19 @@
         <v>6.207E-2</v>
       </c>
       <c r="M29" s="1">
+        <v>3.7920000000000002E-2</v>
+      </c>
+      <c r="N29">
+        <v>9.5869999999999997E-2</v>
+      </c>
+      <c r="O29">
+        <v>1.372E-2</v>
+      </c>
+      <c r="P29" s="1">
         <v>4.5418999999999998E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="B30">
         <v>2016</v>
       </c>
@@ -2289,10 +2567,19 @@
         <v>0.12615999999999999</v>
       </c>
       <c r="M30" s="1">
+        <v>0.11348</v>
+      </c>
+      <c r="N30">
+        <v>0.13885</v>
+      </c>
+      <c r="O30">
+        <v>6.4700000000000001E-3</v>
+      </c>
+      <c r="P30" s="1">
         <v>7.6421799999999998E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>18</v>
       </c>
@@ -2324,10 +2611,19 @@
         <v>0.11744</v>
       </c>
       <c r="M31" s="1">
+        <v>0.10582</v>
+      </c>
+      <c r="N31">
+        <v>0.12906000000000001</v>
+      </c>
+      <c r="O31">
+        <v>5.9300000000000004E-3</v>
+      </c>
+      <c r="P31" s="1">
         <v>8.09637E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B32">
         <v>2017</v>
       </c>
@@ -2362,10 +2658,19 @@
         <v>5.944E-2</v>
       </c>
       <c r="M32" s="1">
+        <v>3.8460000000000001E-2</v>
+      </c>
+      <c r="N32">
+        <v>8.7739999999999999E-2</v>
+      </c>
+      <c r="O32">
+        <v>1.1900000000000001E-2</v>
+      </c>
+      <c r="P32" s="1">
         <v>5.7267000000000004E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="B33">
         <v>2017</v>
       </c>
@@ -2400,10 +2705,19 @@
         <v>0.11744</v>
       </c>
       <c r="M33" s="1">
+        <v>0.10517</v>
+      </c>
+      <c r="N33">
+        <v>0.12970999999999999</v>
+      </c>
+      <c r="O33">
+        <v>6.2599999999999999E-3</v>
+      </c>
+      <c r="P33" s="1">
         <v>7.32622E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>18</v>
       </c>
@@ -2435,10 +2749,19 @@
         <v>0.11083999999999999</v>
       </c>
       <c r="M34" s="1">
+        <v>9.9510000000000001E-2</v>
+      </c>
+      <c r="N34">
+        <v>0.12216</v>
+      </c>
+      <c r="O34">
+        <v>5.7800000000000004E-3</v>
+      </c>
+      <c r="P34" s="1">
         <v>7.8988900000000001E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B35">
         <v>2018</v>
       </c>
@@ -2473,10 +2796,19 @@
         <v>6.4199999999999993E-2</v>
       </c>
       <c r="M35" s="1">
+        <v>4.0230000000000002E-2</v>
+      </c>
+      <c r="N35">
+        <v>9.7189999999999999E-2</v>
+      </c>
+      <c r="O35">
+        <v>1.354E-2</v>
+      </c>
+      <c r="P35" s="1">
         <v>4.9367999999999999E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="B36">
         <v>2018</v>
       </c>
@@ -2511,10 +2843,19 @@
         <v>0.11589000000000001</v>
       </c>
       <c r="M36" s="1">
+        <v>0.10315000000000001</v>
+      </c>
+      <c r="N36">
+        <v>0.12862999999999999</v>
+      </c>
+      <c r="O36">
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="P36" s="1">
         <v>7.1287500000000004E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>18</v>
       </c>
@@ -2546,10 +2887,19 @@
         <v>0.10929</v>
       </c>
       <c r="M37" s="1">
+        <v>9.7629999999999995E-2</v>
+      </c>
+      <c r="N37">
+        <v>0.12094000000000001</v>
+      </c>
+      <c r="O37">
+        <v>5.9500000000000004E-3</v>
+      </c>
+      <c r="P37" s="1">
         <v>7.6224299999999995E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B38">
         <v>2019</v>
       </c>
@@ -2584,10 +2934,19 @@
         <v>6.8680000000000005E-2</v>
       </c>
       <c r="M38" s="1">
+        <v>4.4450000000000003E-2</v>
+      </c>
+      <c r="N38">
+        <v>0.10138999999999999</v>
+      </c>
+      <c r="O38">
+        <v>1.371E-2</v>
+      </c>
+      <c r="P38" s="1">
         <v>5.9242000000000001E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="B39">
         <v>2019</v>
       </c>
@@ -2622,10 +2981,19 @@
         <v>0.13122</v>
       </c>
       <c r="M39" s="1">
+        <v>0.11856</v>
+      </c>
+      <c r="N39">
+        <v>0.14387</v>
+      </c>
+      <c r="O39">
+        <v>6.4599999999999996E-3</v>
+      </c>
+      <c r="P39" s="1">
         <v>8.4518200000000002E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>18</v>
       </c>
@@ -2657,10 +3025,19 @@
         <v>0.12249</v>
       </c>
       <c r="M40" s="1">
+        <v>0.11098</v>
+      </c>
+      <c r="N40">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="O40">
+        <v>5.8700000000000002E-3</v>
+      </c>
+      <c r="P40" s="1">
         <v>9.0442300000000003E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B41">
         <v>2020</v>
       </c>
@@ -2695,10 +3072,19 @@
         <v>5.5230000000000001E-2</v>
       </c>
       <c r="M41" s="1">
+        <v>3.4189999999999998E-2</v>
+      </c>
+      <c r="N41">
+        <v>8.4419999999999995E-2</v>
+      </c>
+      <c r="O41">
+        <v>1.217E-2</v>
+      </c>
+      <c r="P41" s="1">
         <v>4.7393000000000001E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="B42">
         <v>2020</v>
       </c>
@@ -2733,10 +3119,19 @@
         <v>0.12094000000000001</v>
       </c>
       <c r="M42" s="1">
+        <v>0.10822</v>
+      </c>
+      <c r="N42">
+        <v>0.13367000000000001</v>
+      </c>
+      <c r="O42">
+        <v>6.4900000000000001E-3</v>
+      </c>
+      <c r="P42" s="1">
         <v>7.5631900000000002E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>18</v>
       </c>
@@ -2768,10 +3163,19 @@
         <v>0.11645999999999999</v>
       </c>
       <c r="M43" s="1">
+        <v>0.10465000000000001</v>
+      </c>
+      <c r="N43">
+        <v>0.12827</v>
+      </c>
+      <c r="O43">
+        <v>6.0299999999999998E-3</v>
+      </c>
+      <c r="P43" s="1">
         <v>8.0371200000000004E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>18</v>
       </c>
@@ -2797,430 +3201,446 @@
         <v>0.1048</v>
       </c>
       <c r="M44" s="1">
+        <v>0.10184</v>
+      </c>
+      <c r="N44">
+        <v>0.10775999999999999</v>
+      </c>
+      <c r="O44">
+        <v>1.5100000000000001E-3</v>
+      </c>
+      <c r="P44" s="1">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="D1:D44" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Black or African American"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="111.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="111.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>93</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>